<commit_message>
Update homepage redirect logic and add WeChat share functionality
</commit_message>
<xml_diff>
--- a/guestlist.xlsx
+++ b/guestlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weibo/Desktop/spring2025/结婚？/invitation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7D4CF7-B4F8-5948-829D-51B59FCC076C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8FA045-EDAE-AC46-B7A6-5DF7DCE4CD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{CA0BAF00-B0EF-AE45-B93A-A3E19366BAC0}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: add emoji compatibility check for disco ball (🪩/🔵)
</commit_message>
<xml_diff>
--- a/guestlist.xlsx
+++ b/guestlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weibo/Desktop/spring2025/结婚？/invitation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5074805-43B1-9848-B5FB-ACA8E31EEC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDF5247-E7B2-FE40-AE33-67F3008E047B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2120" windowWidth="28040" windowHeight="17440" xr2:uid="{CA0BAF00-B0EF-AE45-B93A-A3E19366BAC0}"/>
+    <workbookView xWindow="3260" yWindow="2100" windowWidth="28040" windowHeight="17440" xr2:uid="{CA0BAF00-B0EF-AE45-B93A-A3E19366BAC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -515,7 +515,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>